<commit_message>
Fixed bug in shove_it().
</commit_message>
<xml_diff>
--- a/Exceptin shove_it() array subscript out of range.xlsx
+++ b/Exceptin shove_it() array subscript out of range.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c51537410c5afe56/Projects/Source/Repos/EdGarrity/SOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{DB738F16-C7E5-4A86-B36A-DE42BB921E71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E8318846-027F-4377-ACD9-1A6F60EF6006}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="8_{DB738F16-C7E5-4A86-B36A-DE42BB921E71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9E22C6E9-7C61-4A25-988A-220405C4DD3A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{7897217C-93DC-4F28-B1F9-89DF7A74A24B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{7897217C-93DC-4F28-B1F9-89DF7A74A24B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2 (2)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
   <si>
     <t>source_position</t>
   </si>
@@ -82,6 +84,54 @@
   </si>
   <si>
     <t>Program</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>--&gt;</t>
+  </si>
+  <si>
+    <t>top - 1 --&gt; top - 1 + len</t>
+  </si>
+  <si>
+    <t>len</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>top - 1</t>
+  </si>
+  <si>
+    <t>top - 1 + len</t>
+  </si>
+  <si>
+    <t>do while</t>
+  </si>
+  <si>
+    <t>Iterate</t>
+  </si>
+  <si>
+    <t>++</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>&lt; length</t>
+  </si>
+  <si>
+    <t>&lt; (top - destination_index)</t>
   </si>
 </sst>
 </file>
@@ -117,8 +167,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBAF31AD-FD35-47EB-8DDF-0FE6BC2AAD84}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="194" zoomScaleNormal="194" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A11" zoomScale="194" zoomScaleNormal="194" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -649,4 +703,1318 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C8E82A3-5101-493B-9DAF-DC2A9F368854}">
+  <dimension ref="A1:L26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>20-A2</f>
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>20-E2</f>
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B22" si="0">20-A3</f>
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <f>C2+1</f>
+        <v>101</v>
+      </c>
+      <c r="E3">
+        <f>E2+1</f>
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F22" si="1">20-E3</f>
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f t="shared" ref="A4:A20" si="2">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C22" si="3">C3+1</f>
+        <v>102</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E20" si="4">E3+1</f>
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="3"/>
+        <v>103</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="3"/>
+        <v>104</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="3"/>
+        <v>105</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="G7">
+        <f>G6+1</f>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="3"/>
+        <v>106</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ref="G8:G26" si="5">G7+1</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="3"/>
+        <v>107</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="5"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="3"/>
+        <v>108</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="5"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="3"/>
+        <v>109</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="5"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f>A11+1</f>
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="3"/>
+        <v>110</v>
+      </c>
+      <c r="E12">
+        <f>E11+1</f>
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="5"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="3"/>
+        <v>111</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ref="E13:E26" si="6">E12+1</f>
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="5"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="3"/>
+        <v>112</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="5"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="3"/>
+        <v>113</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="5"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="3"/>
+        <v>114</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="5"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="3"/>
+        <v>115</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="5"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="3"/>
+        <v>116</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="5"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="3"/>
+        <v>117</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="5"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="3"/>
+        <v>118</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="5"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" ref="A21:A22" si="7">A20+1</f>
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="3"/>
+        <v>119</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="6"/>
+        <v>19</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="5"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="5"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <f t="shared" si="6"/>
+        <v>21</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="5"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <f t="shared" si="6"/>
+        <v>22</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="5"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <f t="shared" si="6"/>
+        <v>23</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="5"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="5"/>
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F87EA4DA-80BE-4AE1-AF00-D981FF96F3E9}">
+  <dimension ref="A1:L26"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>20-A2</f>
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>20-E2</f>
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>117</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B22" si="0">20-A3</f>
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <f>E2+1</f>
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F22" si="1">20-E3</f>
+        <v>19</v>
+      </c>
+      <c r="G3">
+        <v>118</v>
+      </c>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f t="shared" ref="A4:A20" si="2">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E20" si="3">E3+1</f>
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="G4">
+        <v>119</v>
+      </c>
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="G5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <f>C6+1</f>
+        <v>101</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="G7">
+        <f>G6+1</f>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:C26" si="4">C7+1</f>
+        <v>102</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ref="G8:G22" si="5">G7+1</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="4"/>
+        <v>103</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="5"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="4"/>
+        <v>104</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="5"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="4"/>
+        <v>105</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="5"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f>A11+1</f>
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="4"/>
+        <v>106</v>
+      </c>
+      <c r="E12">
+        <f>E11+1</f>
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="5"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" ref="A13:A26" si="6">A12+1</f>
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="4"/>
+        <v>107</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ref="E13:E26" si="7">E12+1</f>
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="5"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="4"/>
+        <v>108</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="5"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="4"/>
+        <v>109</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="7"/>
+        <v>13</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="5"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="4"/>
+        <v>110</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="5"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="4"/>
+        <v>111</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="5"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="4"/>
+        <v>112</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="5"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="4"/>
+        <v>113</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="7"/>
+        <v>17</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="5"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="4"/>
+        <v>114</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="7"/>
+        <v>18</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="5"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" si="6"/>
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="4"/>
+        <v>115</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="7"/>
+        <v>19</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="5"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="4"/>
+        <v>116</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="5"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" si="6"/>
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="4"/>
+        <v>117</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="7"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f t="shared" si="6"/>
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="4"/>
+        <v>118</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="7"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <f t="shared" si="6"/>
+        <v>23</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="4"/>
+        <v>119</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="7"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="4"/>
+        <v>120</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="7"/>
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>